<commit_message>
added slides for update
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/batch_CD_CDART/1283_AQBs_gids_hitdata_v1.xlsx
+++ b/flag/AQB_classification/batch_CD_CDART/1283_AQBs_gids_hitdata_v1.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/bioinfRhints/flag/AQB_classification/batch_CD_CDART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{318CECF5-5058-C247-B6D0-EB11909D4785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B8A9DF00-F3EF-4840-A0D2-D8A609DF1034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="4000" windowWidth="27240" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="1283_AQBs_gids_hitdata" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1283_AQBs_gids_hitdata'!$A$1:$L$1327</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -4939,10 +4942,10 @@
   <dimension ref="A1:L1327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C1274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C1258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="J1272" sqref="J1272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>